<commit_message>
Final pre-production edit for LM-003
</commit_message>
<xml_diff>
--- a/LM-003-Production/Project Outputs for LM-003/LM-003.xlsx
+++ b/LM-003-Production/Project Outputs for LM-003/LM-003.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zls\Desktop\Land_Meter_PCB\LM-003-Production\Project Outputs for LM-003\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="9885" xr2:uid="{AD373C22-AB65-4FF5-8D25-A85961524203}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="9885" xr2:uid="{A5BF10F5-50D9-437A-A36D-C11ED5EE92D5}"/>
   </bookViews>
   <sheets>
     <sheet name="LM-003" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="144">
   <si>
     <t>Comment</t>
   </si>
@@ -66,274 +71,229 @@
     <t>ComponentLink4Description</t>
   </si>
   <si>
-    <t>MS621FE-FL11E</t>
-  </si>
-  <si>
-    <t>MS Lihium Rechargeable Battery, 3 V, -20 to 60 degC, Tray</t>
-  </si>
-  <si>
-    <t>BT1</t>
-  </si>
-  <si>
-    <t>SEIK-MS621FE-FL11E-2_V</t>
-  </si>
-  <si>
-    <t>SeikoInstruments</t>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 10V X7R 0402</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>CAPC0402(1005)60_L</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>Cut Tape (CT)</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Tray</t>
-  </si>
-  <si>
-    <t>Real Time Clock.SchDoc</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 10V X7R 0402</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>CAPC0402(1005)60_L</t>
-  </si>
-  <si>
-    <t>Murata Electronics North America</t>
-  </si>
-  <si>
-    <t>0402 (1005 Metric)</t>
-  </si>
-  <si>
-    <t>Cut Tape (CT)</t>
-  </si>
-  <si>
     <t>BBB Headers.SchDoc</t>
   </si>
   <si>
     <t>http://www.murata.com/~/media/webrenewal/support/library/catalog/products/capacitor/mlcc/c02e.ashx?la=en-us</t>
   </si>
   <si>
-    <t>CAP 100nF 25V 0805(2012)</t>
-  </si>
-  <si>
-    <t>CAP 100nF 25V -20% to +80% 0805 (2012 Metric) Thickness 1mm SMD</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>CAPC0805(2012)100_N</t>
+    <t>Lite-On LTST-S220KGKT Green LED, 571 nm 2012 (0805) Side View, Rectangle Lens SMD package</t>
+  </si>
+  <si>
+    <t>DS1, DS2</t>
+  </si>
+  <si>
+    <t>0805C_L</t>
+  </si>
+  <si>
+    <t>Vishay / Lite-On</t>
+  </si>
+  <si>
+    <t>Tape and Reel</t>
+  </si>
+  <si>
+    <t>Power.SchDoc</t>
+  </si>
+  <si>
+    <t>https://datasheet.ciiva.com/11775/0900766b80dc0b70-11775441.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.ciiva.com/2110/s-110-ltst-s220kgkt-2110069.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.ciiva.com/12400/100-ltst-s220kgkt-59602-12400886.pdf</t>
+  </si>
+  <si>
+    <t>LTST-C19HE1WT</t>
+  </si>
+  <si>
+    <t>LED Tri-Color Blue/Green/Red, 5 V, -20 to 80 degC, 4-Pin SMD, RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>DS3</t>
+  </si>
+  <si>
+    <t>LTST-C19HE1WT-4_V</t>
+  </si>
+  <si>
+    <t>Lite-On</t>
+  </si>
+  <si>
+    <t>RS232.SchDoc</t>
+  </si>
+  <si>
+    <t>Visible Name Value Type    False Description Lite-On LTST-S220KRKT Red LED, 631 nm 2012 (0805) Side View, Rectangle Lens SMD package STRING</t>
+  </si>
+  <si>
+    <t>DS4, DS5, DS6, DS7</t>
+  </si>
+  <si>
+    <t>heater_control.SchDoc</t>
+  </si>
+  <si>
+    <t>https://datasheet.ciiva.com/2110/s-110-ltst-s220krkt-2110132.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.ciiva.com/2110/s-110-ltst-s220krkt-2110133.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.ciiva.com/12403/lite-on-ltst-s220krkt-187389-12403798.pdf</t>
+  </si>
+  <si>
+    <t>SLW-108-01-G-D</t>
+  </si>
+  <si>
+    <t>P1, P2</t>
+  </si>
+  <si>
+    <t>Header 3</t>
+  </si>
+  <si>
+    <t>Header, 3-Pin</t>
+  </si>
+  <si>
+    <t>P3, P4</t>
+  </si>
+  <si>
+    <t>HDR1X3</t>
+  </si>
+  <si>
+    <t>Connectors.SchDoc</t>
+  </si>
+  <si>
+    <t>IPL1-105-01-F-S-K</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>Header 7</t>
+  </si>
+  <si>
+    <t>Header, 7-Pin</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>HDR1X7</t>
+  </si>
+  <si>
+    <t>SLW-105-01-G-D</t>
+  </si>
+  <si>
+    <t>CONN RCPT .100" 10POS DUAL GOLD</t>
+  </si>
+  <si>
+    <t>P7, P8</t>
+  </si>
+  <si>
+    <t>Samtec Inc.</t>
+  </si>
+  <si>
+    <t>Bulk</t>
+  </si>
+  <si>
+    <t>http://suddendocs.samtec.com/prints/slw-1xx-01-x-x-mkt.pdf</t>
+  </si>
+  <si>
+    <t>FSI-120-03-G-D-E-AB</t>
+  </si>
+  <si>
+    <t>1MM SINGLE ELEMENT INTERFACE</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>Tube</t>
+  </si>
+  <si>
+    <t>http://suddendocs.samtec.com/prints/fsi-1xx-03-x-d-x-xx-xx-mkt.pdf</t>
+  </si>
+  <si>
+    <t>Header 100 mil (2.54 mm)</t>
+  </si>
+  <si>
+    <t>CABLE USB SERIAL 3.3V 2MM HEADER</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>HDR1X6</t>
+  </si>
+  <si>
+    <t>http://www.ftdichip.com/Support/Documents/DataSheets/Cables/DS_TTL-232R_CABLES.pdf</t>
+  </si>
+  <si>
+    <t>IPL1-112-01-F-S-K</t>
+  </si>
+  <si>
+    <t>IPL1-112-01-F-D-K</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>https://datasheet.ciiva.com/9444/ipl1-9444389.pdf</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R1, R4, R6, R8</t>
+  </si>
+  <si>
+    <t>RESC0805(2012)_L</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
   </si>
   <si>
     <t>0805 (2012 Metric)</t>
   </si>
   <si>
-    <t>http://www.murata.com/~/media/webrenewal/support/library/catalog/products/capacitor/mlcc/c02e.ashx</t>
-  </si>
-  <si>
-    <t>CAP 1uF 25V 0805(2012)</t>
-  </si>
-  <si>
-    <t>CAP 1uF 25V ±10% 0805 (2012 Metric) Thickness 1mm SMD</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>CAPC0805(2012)100_M</t>
-  </si>
-  <si>
-    <t>Lite-On LTST-S220KGKT Green LED, 571 nm 2012 (0805) Side View, Rectangle Lens SMD package</t>
-  </si>
-  <si>
-    <t>DS1, DS2</t>
-  </si>
-  <si>
-    <t>0805C_L</t>
-  </si>
-  <si>
-    <t>Vishay / Lite-On</t>
-  </si>
-  <si>
-    <t>Tape and Reel</t>
-  </si>
-  <si>
-    <t>Power.SchDoc</t>
-  </si>
-  <si>
-    <t>https://datasheet.ciiva.com/11775/0900766b80dc0b70-11775441.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.ciiva.com/2110/s-110-ltst-s220kgkt-2110069.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.ciiva.com/12400/100-ltst-s220kgkt-59602-12400886.pdf</t>
-  </si>
-  <si>
-    <t>LTST-C19HE1WT</t>
-  </si>
-  <si>
-    <t>LED Tri-Color Blue/Green/Red, 5 V, -20 to 80 degC, 4-Pin SMD, RoHS, Tape and Reel</t>
-  </si>
-  <si>
-    <t>DS3</t>
-  </si>
-  <si>
-    <t>LTST-C19HE1WT-4_V</t>
-  </si>
-  <si>
-    <t>Lite-On</t>
-  </si>
-  <si>
-    <t>RS232.SchDoc</t>
-  </si>
-  <si>
-    <t>Visible Name Value Type    False Description Lite-On LTST-S220KRKT Red LED, 631 nm 2012 (0805) Side View, Rectangle Lens SMD package STRING</t>
-  </si>
-  <si>
-    <t>DS4, DS5, DS6, DS7</t>
-  </si>
-  <si>
-    <t>heater_control.SchDoc</t>
-  </si>
-  <si>
-    <t>https://datasheet.ciiva.com/2110/s-110-ltst-s220krkt-2110132.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.ciiva.com/2110/s-110-ltst-s220krkt-2110133.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.ciiva.com/12403/lite-on-ltst-s220krkt-187389-12403798.pdf</t>
-  </si>
-  <si>
-    <t>SLW-108-01-G-D</t>
-  </si>
-  <si>
-    <t>P1, P2</t>
-  </si>
-  <si>
-    <t>Header 3</t>
-  </si>
-  <si>
-    <t>Header, 3-Pin</t>
-  </si>
-  <si>
-    <t>P3, P4</t>
-  </si>
-  <si>
-    <t>HDR1X3</t>
-  </si>
-  <si>
-    <t>Connectors.SchDoc</t>
-  </si>
-  <si>
-    <t>IPL1-105-01-F-S-K</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>Header 7</t>
-  </si>
-  <si>
-    <t>Header, 7-Pin</t>
-  </si>
-  <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>HDR1X7</t>
-  </si>
-  <si>
-    <t>SLW-105-01-G-D</t>
-  </si>
-  <si>
-    <t>CONN RCPT .100" 10POS DUAL GOLD</t>
-  </si>
-  <si>
-    <t>P7, P8</t>
-  </si>
-  <si>
-    <t>Samtec Inc.</t>
-  </si>
-  <si>
-    <t>Bulk</t>
-  </si>
-  <si>
-    <t>http://suddendocs.samtec.com/prints/slw-1xx-01-x-x-mkt.pdf</t>
-  </si>
-  <si>
-    <t>FSI-120-03-G-D-E-AB</t>
-  </si>
-  <si>
-    <t>1MM SINGLE ELEMENT INTERFACE</t>
-  </si>
-  <si>
-    <t>P9</t>
-  </si>
-  <si>
-    <t>Tube</t>
-  </si>
-  <si>
-    <t>http://suddendocs.samtec.com/prints/fsi-1xx-03-x-d-x-xx-xx-mkt.pdf</t>
-  </si>
-  <si>
-    <t>Header 100 mil (2.54 mm)</t>
-  </si>
-  <si>
-    <t>CABLE USB SERIAL 3.3V 2MM HEADER</t>
-  </si>
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>HDR1X6</t>
-  </si>
-  <si>
-    <t>http://www.ftdichip.com/Support/Documents/DataSheets/Cables/DS_TTL-232R_CABLES.pdf</t>
-  </si>
-  <si>
-    <t>IPL1-112-01-F-S-K</t>
-  </si>
-  <si>
-    <t>IPL1-112-01-F-D-K</t>
-  </si>
-  <si>
-    <t>P11</t>
-  </si>
-  <si>
-    <t>Samtec</t>
-  </si>
-  <si>
-    <t>https://datasheet.ciiva.com/9444/ipl1-9444389.pdf</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>R1, R4, R7, R9</t>
-  </si>
-  <si>
-    <t>RESC0805(2012)_L</t>
-  </si>
-  <si>
-    <t>Vishay Dale</t>
-  </si>
-  <si>
     <t>Digi-Reel®</t>
   </si>
   <si>
     <t>http://www.vishay.com/docs/20008/dcrcw.pdf</t>
   </si>
   <si>
+    <t>10k</t>
+  </si>
+  <si>
     <t>R2</t>
   </si>
   <si>
-    <t>RESC0805(2012)_M</t>
+    <t>RESC0402(1005)_M</t>
   </si>
   <si>
     <t>RES SMD 1K OHM 1% 1/8W 0805</t>
@@ -354,55 +314,52 @@
     <t>http://www.vishay.com/docs/20043/crcwhpe3.pdf</t>
   </si>
   <si>
-    <t>RES SMD 4.7K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
     <t>RES SMD 4.99K OHM 1% 1/8W 0805</t>
   </si>
   <si>
-    <t>R8, R10</t>
-  </si>
-  <si>
-    <t>RES SMD 10k OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>RES SMD TBD OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>RESC0805(2012)_N</t>
-  </si>
-  <si>
-    <t>R12, R13</t>
-  </si>
-  <si>
-    <t>BBB Headers.SchDoc, Real Time Clock.SchDoc</t>
-  </si>
-  <si>
-    <t>RES SMD 100 OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>R14, R15, R16, R18</t>
+    <t>R7, R9</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>R10, R11</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>R13, R17, R18, R19, R20, R21, R27, R28</t>
+  </si>
+  <si>
+    <t>BBB Headers.SchDoc, RS232.SchDoc, RS232.SchDoc, RS232.SchDoc, RS232.SchDoc, RS232.SchDoc, RS232.SchDoc, BBB Headers.SchDoc</t>
   </si>
   <si>
     <t>DNP</t>
   </si>
   <si>
-    <t>RES SMD 1K OHM 1% 1/2W 0805</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>R20, R21, R22, R23</t>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>19.1k</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>4.99k</t>
+  </si>
+  <si>
+    <t>R22, R23, R24, R25, R26</t>
+  </si>
+  <si>
+    <t>heater_control.SchDoc, heater_control.SchDoc, heater_control.SchDoc, heater_control.SchDoc, Power.SchDoc</t>
   </si>
   <si>
     <t>BBB</t>
@@ -468,25 +425,19 @@
     <t>http://www.analog.com/static/imported-files/data_sheets/ADG1608_1609.pdf</t>
   </si>
   <si>
-    <t>DS1394U-33+</t>
-  </si>
-  <si>
-    <t>SPI Real-Time Clock with Trickle Charger, 3.3V, 10-Pin uSOP, -40 to 85 degC, Pb-Free</t>
+    <t>MS563702BA03-50</t>
+  </si>
+  <si>
+    <t>Low Voltage Barometric Pressure Sensor, 1.5 to 3.6 V, -40 to 85 degC, 4-Pin SMD, RoHS, Tape and Reel</t>
   </si>
   <si>
     <t>U4</t>
   </si>
   <si>
-    <t>U10+2_N</t>
-  </si>
-  <si>
-    <t>Maxim Integrated</t>
-  </si>
-  <si>
-    <t>10-TFSOP, 10-MSOP (0.118", 3.00mm Width)</t>
-  </si>
-  <si>
-    <t>http://datasheets.maximintegrated.com/en/ds/DS1390-DS1394.pdf</t>
+    <t>TECO-MS563702BA03-50_V</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
   </si>
   <si>
     <t>OPA4188AIPWR</t>
@@ -505,12 +456,6 @@
   </si>
   <si>
     <t>http://www.ti.com/lit/ds/symlink/opa4188.pdf</t>
-  </si>
-  <si>
-    <t>AB26TRQ-32.768KHZ-T</t>
-  </si>
-  <si>
-    <t>X1</t>
   </si>
 </sst>
 </file>
@@ -893,17 +838,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54660A6-8502-4045-A68F-20A0FE8FE426}">
-  <dimension ref="A1:O34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD3D2A4-7D44-484E-A560-B18178D8E5C7}">
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="5.85546875" customWidth="1"/>
     <col min="6" max="9" width="3.28515625" customWidth="1"/>
     <col min="10" max="10" width="4.5703125" customWidth="1"/>
@@ -980,1535 +927,1303 @@
         <v>21</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I3" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I6" s="3">
         <v>2</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I7" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="I8" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>60</v>
+        <v>131</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>61</v>
+        <v>132</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I9" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I10" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I11" s="3">
         <v>1</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="K11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="N11" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I12" s="3">
         <v>1</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I13" s="3">
         <v>2</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I14" s="3">
         <v>1</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I15" s="3">
         <v>1</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I16" s="3">
         <v>1</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I17" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>102</v>
+        <v>31</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I18" s="3">
         <v>1</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>99</v>
+        <v>136</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I19" s="3">
         <v>1</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
       <c r="I20" s="3">
         <v>1</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>20</v>
+        <v>122</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>20</v>
+        <v>124</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>20</v>
+        <v>138</v>
       </c>
       <c r="I21" s="3">
         <v>1</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>20</v>
+        <v>142</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I22" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I23" s="3">
         <v>1</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>30</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I24" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I25" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>121</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>126</v>
+        <v>47</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I27" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>20</v>
+        <v>105</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I28" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>130</v>
+        <v>41</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>129</v>
+        <v>27</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>131</v>
+        <v>28</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I29" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I30" s="3">
-        <v>1</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="I31" s="3">
-        <v>1</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32" s="3">
-        <v>1</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O32" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="I33" s="3">
-        <v>1</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I34" s="3">
-        <v>1</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:O29">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>